<commit_message>
BasicApp: update business data file
</commit_message>
<xml_diff>
--- a/basic-application/basic-application-core/src/main/resources/init/business_data.xlsx
+++ b/basic-application/basic-application-core/src/main/resources/init/business_data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -197,6 +197,18 @@
   </si>
   <si>
     <t xml:space="preserve">corinne.fagno@kobalt.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anaïs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rouvière</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arouviere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anais.rouviere@kobalt.fr</t>
   </si>
 </sst>
 </file>
@@ -361,7 +373,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -371,7 +383,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.01171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.28"/>
@@ -432,7 +444,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -442,7 +454,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.01171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -510,7 +522,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -520,13 +532,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.01171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.57"/>
@@ -608,24 +620,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.57"/>
@@ -919,6 +931,35 @@
         <v>2</v>
       </c>
       <c r="I10" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" s="0" t="s">
         <v>22</v>
       </c>
     </row>
@@ -933,6 +974,7 @@
     <hyperlink ref="E8" r:id="rId7" display="mathieu.palley@kobalt.fr"/>
     <hyperlink ref="E9" r:id="rId8" display="alexandre.wallois@kobalt.fr"/>
     <hyperlink ref="E10" r:id="rId9" display="corinne.fagno@kobalt.fr"/>
+    <hyperlink ref="E11" r:id="rId10" display="anais.rouviere@kobalt.fr"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -942,7 +984,7 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BasicApp: use kobalt email address for admin user
</commit_message>
<xml_diff>
--- a/basic-application/basic-application-core/src/main/resources/init/business_data.xlsx
+++ b/basic-application/basic-application-core/src/main/resources/init/business_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Authority" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -79,13 +79,16 @@
     <t xml:space="preserve">locale</t>
   </si>
   <si>
-    <t xml:space="preserve">Administrateur</t>
+    <t xml:space="preserve">Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kobalt</t>
   </si>
   <si>
     <t xml:space="preserve">admin</t>
   </si>
   <si>
-    <t xml:space="preserve">admin@example.com</t>
+    <t xml:space="preserve">interne-qualif@kobalt.fr</t>
   </si>
   <si>
     <t xml:space="preserve">kobalt</t>
@@ -383,7 +386,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.28"/>
@@ -454,7 +457,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -528,16 +531,16 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.58"/>
@@ -573,7 +576,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -581,16 +584,16 @@
         <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>1</v>
@@ -599,12 +602,12 @@
         <v>4</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="admin@example.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="interne-qualif@kobalt.fr"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -626,11 +629,11 @@
   </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.59"/>
@@ -678,19 +681,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>2</v>
@@ -699,7 +702,7 @@
         <v>2</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -707,19 +710,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>2</v>
@@ -728,7 +731,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -736,19 +739,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>2</v>
@@ -757,7 +760,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -765,19 +768,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>2</v>
@@ -786,7 +789,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -794,19 +797,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>2</v>
@@ -815,7 +818,7 @@
         <v>2</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,19 +826,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>2</v>
@@ -844,7 +847,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -852,19 +855,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>2</v>
@@ -873,7 +876,7 @@
         <v>2</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -881,19 +884,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>2</v>
@@ -902,7 +905,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -910,19 +913,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>2</v>
@@ -931,7 +934,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -939,19 +942,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>2</v>
@@ -960,7 +963,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BasicApp: update business data user disabled
</commit_message>
<xml_diff>
--- a/basic-application/basic-application-core/src/main/resources/init/business_data.xlsx
+++ b/basic-application/basic-application-core/src/main/resources/init/business_data.xlsx
@@ -242,7 +242,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -270,11 +270,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -324,15 +319,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -345,6 +340,22 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0000FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -407,7 +418,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -419,47 +430,47 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -478,7 +489,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -490,54 +501,54 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -556,7 +567,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -568,71 +579,71 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="6.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -654,412 +665,412 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="244" min="11" style="0" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="244" min="11" style="1" width="10.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J2" s="0" t="s">
+      <c r="H2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J3" s="0" t="s">
+      <c r="H3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J4" s="0" t="s">
+      <c r="H4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J5" s="0" t="s">
+      <c r="H5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J6" s="0" t="s">
+      <c r="H6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J7" s="0" t="s">
+      <c r="H7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J8" s="0" t="s">
+      <c r="H8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J9" s="0" t="s">
+      <c r="H9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="G10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J10" s="0" t="s">
+      <c r="H10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="G11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J12" s="0" t="s">
+      <c r="H12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update users in business_data.xlsx
</commit_message>
<xml_diff>
--- a/basic-application/basic-application-core/src/main/resources/init/business_data.xlsx
+++ b/basic-application/basic-application-core/src/main/resources/init/business_data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="78">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -233,6 +233,30 @@
   </si>
   <si>
     <t xml:space="preserve">chloe.baffert-buivan@kobalt.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aurélien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jolivet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajolivet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aurelien.jolivet@kobalt.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vincent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vweber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vincent.weber@kobalt.fr</t>
   </si>
 </sst>
 </file>
@@ -669,10 +693,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1074,6 +1098,70 @@
         <v>23</v>
       </c>
     </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="laurent.almeras@kobalt.fr"/>
@@ -1087,6 +1175,8 @@
     <hyperlink ref="E10" r:id="rId9" display="corinne.fagno@kobalt.fr"/>
     <hyperlink ref="E11" r:id="rId10" display="anais.rouviere@kobalt.fr"/>
     <hyperlink ref="E12" r:id="rId11" display="chloe.baffert-buivan@kobalt.fr"/>
+    <hyperlink ref="E13" r:id="rId12" display="aurelien.jolivet@kobalt.fr"/>
+    <hyperlink ref="E14" r:id="rId13" display="vincent.weber@kobalt.fr"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1096,7 +1186,7 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>